<commit_message>
Update for EA 23.188 Stable. Harvesting, replanting, shared containers, and equalize have been removed due to updates and bugs. Add a new option for residents to match planted seed level to the player’s farming skill level.
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -85,16 +85,16 @@
     <t xml:space="preserve">tooltip01</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable or disable the use of fertilizer.
-Set to 'true' to enable fertilizer, or 'false' to disable it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">肥料の使用を有効または無効にします。
-'true' に設定すると肥料が有効になり、'false' に設定すると無効になります。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">启用或禁用肥料的使用。
-设置为 'true' 启用肥料，设置为 'false' 禁用肥料。</t>
+    <t xml:space="preserve">Enable or disable residents applying fertilizer to crops.
+Set to 'true' to allow residents to apply fertilizer during farming, or 'false' to prevent them from using fertilizer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">住人が作物に肥料を施すかどうかを設定します。
+'true' に設定すると住人が農作業中に肥料を施し、'false' では施しません。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用居民为作物施肥。
+设置为 'true' 时，居民会在农作时施肥；设置为 'false' 时，他们不会施肥。</t>
   </si>
   <si>
     <t xml:space="preserve">toggle02</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">toggle03</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable Equalize Plants</t>
+    <t xml:space="preserve">Enable Seed Level Match</t>
   </si>
   <si>
     <t xml:space="preserve">植物の均等化を有効化</t>
@@ -139,101 +139,16 @@
     <t xml:space="preserve">tooltip03</t>
   </si>
   <si>
-    <t xml:space="preserve">Enable or disable the equalization of plants in neighboring tiles.
-Equalization means that plants in neighboring tiles will share the same growth level and seed type if they match certain conditions.
-Set to 'true' to enable equalization, or 'false' to disable it.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">隣接するタイルの植物を均等化するかどうかを有効または無効にします。
-均等化とは、特定の条件を満たす場合、隣接するタイルの植物が同じ成長レベルや種子の種類を共有することを意味します。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'true' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">に設定すると均等化が有効になり、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'false' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">に設定すると無効になります。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">启用或禁用邻近地块植物的均衡化。
-均衡化意味着如果满足某些条件，邻近地块的植物将共享相同的生长水平和种子类型。
-设置为 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'true' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">启用均衡化，设置为 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'false' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">禁用均衡化。</t>
-    </r>
+    <t xml:space="preserve">Enable or disable residents setting the planted seed level to match the player's farming skill level.
+Set to 'true' to have residents adjust seeds to the player's farming skill level when planting, or 'false' to leave the seed level unchanged.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">住人が植え付け時に種のレベルをプレイヤーの農業スキルレベルに合わせるかどうかを設定します。
+'true' に設定すると、住人が種を植える際にプレイヤーの農業スキルレベルに設定されます。'false' では変更しません。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用居民在播种时将种子等级匹配为玩家的农业技能等级。
+设置为 'true' 时，居民在播种时会将种子等级设为玩家的农业技能等级；设置为 'false' 则不更改。</t>
   </si>
 </sst>
 </file>
@@ -243,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,11 +185,6 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,10 +243,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,10 +372,10 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="65.95"/>
@@ -520,7 +426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -534,7 +440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -548,7 +454,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -562,7 +468,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -576,7 +482,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -590,17 +496,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -611,10 +517,10 @@
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>